<commit_message>
Documentation améliorée et create_one_onglet_by_participant passée dans la classe FIle
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_column_set_answer.xlsx
+++ b/fichiers_xls/test_column_set_answer.xlsx
@@ -462,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:AQ15"/>
+  <dimension ref="A1:BX15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -700,6 +700,171 @@
           <t>group3</t>
         </is>
       </c>
+      <c r="AR2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AS2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AT2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AU2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AV2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AW2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AX2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AY2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AZ2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BA2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BB2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BC2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BD2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BE2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BF2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BG2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BH2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BI2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BJ2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BK2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BL2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BM2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BN2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BO2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BP2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BQ2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BR2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BS2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BT2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BU2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BV2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BW2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BX2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="16.05" customHeight="1" s="4">
       <c r="A3" s="3" t="inlineStr">
@@ -915,6 +1080,171 @@
           <t>group1</t>
         </is>
       </c>
+      <c r="AR3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AS3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AT3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AU3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AV3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AW3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AX3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AY3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AZ3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BA3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BB3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BC3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BD3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BE3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BF3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BG3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BH3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BI3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BJ3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BK3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BL3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BM3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BN3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BO3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BP3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BQ3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BR3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BS3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BT3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BU3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BV3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BW3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BX3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="16.05" customHeight="1" s="4">
       <c r="A4" s="3" t="inlineStr">
@@ -1130,6 +1460,171 @@
           <t>group3</t>
         </is>
       </c>
+      <c r="AR4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AS4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AT4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AU4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AV4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AW4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AX4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AY4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AZ4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BA4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BB4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BC4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BD4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BE4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BF4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BG4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BH4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BI4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BJ4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BK4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BL4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BM4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BN4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BO4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BP4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BQ4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BR4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BS4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BT4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BU4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BV4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BW4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BX4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="16.05" customHeight="1" s="4">
       <c r="A5" s="3" t="inlineStr">
@@ -1345,6 +1840,171 @@
           <t>group3</t>
         </is>
       </c>
+      <c r="AR5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AS5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AT5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AU5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AV5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AW5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AX5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AY5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AZ5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BA5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BB5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BC5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BD5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BE5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BF5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BG5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BH5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BI5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BJ5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BK5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BL5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BM5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BN5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BO5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BP5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BQ5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BR5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BS5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BT5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BU5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BV5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BW5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BX5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="16.05" customHeight="1" s="4">
       <c r="A6" s="3" t="inlineStr">
@@ -1560,6 +2220,171 @@
           <t>group1</t>
         </is>
       </c>
+      <c r="AR6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AS6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AT6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AU6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AV6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AW6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AX6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AY6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AZ6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BA6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BB6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BC6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BD6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BE6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BF6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BG6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BH6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BI6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BJ6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BK6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BL6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BM6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BN6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BO6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BP6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BQ6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BR6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BS6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BT6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BU6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BV6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BW6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BX6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="16.05" customHeight="1" s="4">
       <c r="A7" s="3" t="inlineStr">
@@ -1775,6 +2600,171 @@
           <t>group1</t>
         </is>
       </c>
+      <c r="AR7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AS7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AT7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AU7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AV7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AW7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AX7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AY7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AZ7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BA7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BB7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BC7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BD7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BE7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BF7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BG7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BH7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BI7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BJ7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BK7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BL7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BM7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BN7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BO7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BP7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BQ7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BR7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BS7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BT7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BU7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BV7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BW7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BX7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="16.05" customHeight="1" s="4">
       <c r="A8" s="3" t="inlineStr">
@@ -1990,6 +2980,171 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="AR8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AS8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AT8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AU8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AV8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AW8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AX8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AY8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AZ8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BA8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BB8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BC8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BD8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BE8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BF8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BG8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BH8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BI8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BJ8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BK8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BL8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BM8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BN8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BO8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BP8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BQ8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BR8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BS8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BT8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BU8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BV8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BW8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BX8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="16.05" customHeight="1" s="4">
       <c r="A9" s="3" t="inlineStr">
@@ -2201,6 +3356,171 @@
         </is>
       </c>
       <c r="AQ9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AR9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AS9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AT9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AU9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AV9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AW9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AX9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AY9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AZ9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BA9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BB9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BC9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BD9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BE9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BF9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BG9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BH9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BI9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BJ9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BK9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BL9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BM9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BN9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BO9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BP9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BQ9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BR9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BS9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BT9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BU9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BV9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BW9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BX9" s="3" t="inlineStr">
         <is>
           <t>group2</t>
         </is>
@@ -2254,6 +3574,39 @@
       <c r="AO10" s="3" t="inlineStr"/>
       <c r="AP10" s="3" t="inlineStr"/>
       <c r="AQ10" s="3" t="inlineStr"/>
+      <c r="AR10" s="3" t="inlineStr"/>
+      <c r="AS10" s="3" t="inlineStr"/>
+      <c r="AT10" s="3" t="inlineStr"/>
+      <c r="AU10" s="3" t="inlineStr"/>
+      <c r="AV10" s="3" t="inlineStr"/>
+      <c r="AW10" s="3" t="inlineStr"/>
+      <c r="AX10" s="3" t="inlineStr"/>
+      <c r="AY10" s="3" t="inlineStr"/>
+      <c r="AZ10" s="3" t="inlineStr"/>
+      <c r="BA10" s="3" t="inlineStr"/>
+      <c r="BB10" s="3" t="inlineStr"/>
+      <c r="BC10" s="3" t="inlineStr"/>
+      <c r="BD10" s="3" t="inlineStr"/>
+      <c r="BE10" s="3" t="inlineStr"/>
+      <c r="BF10" s="3" t="inlineStr"/>
+      <c r="BG10" s="3" t="inlineStr"/>
+      <c r="BH10" s="3" t="inlineStr"/>
+      <c r="BI10" s="3" t="inlineStr"/>
+      <c r="BJ10" s="3" t="inlineStr"/>
+      <c r="BK10" s="3" t="inlineStr"/>
+      <c r="BL10" s="3" t="inlineStr"/>
+      <c r="BM10" s="3" t="inlineStr"/>
+      <c r="BN10" s="3" t="inlineStr"/>
+      <c r="BO10" s="3" t="inlineStr"/>
+      <c r="BP10" s="3" t="inlineStr"/>
+      <c r="BQ10" s="3" t="inlineStr"/>
+      <c r="BR10" s="3" t="inlineStr"/>
+      <c r="BS10" s="3" t="inlineStr"/>
+      <c r="BT10" s="3" t="inlineStr"/>
+      <c r="BU10" s="3" t="inlineStr"/>
+      <c r="BV10" s="3" t="inlineStr"/>
+      <c r="BW10" s="3" t="inlineStr"/>
+      <c r="BX10" s="3" t="inlineStr"/>
     </row>
     <row r="11" ht="16.05" customHeight="1" s="4">
       <c r="A11" s="3" t="inlineStr">
@@ -2469,6 +3822,171 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="AR11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AS11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AT11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AU11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AV11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AW11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AX11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AY11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AZ11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BA11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BB11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BC11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BD11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BE11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BF11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BG11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BH11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BI11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BJ11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BK11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BL11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BM11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BN11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BO11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BP11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BQ11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BR11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BS11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BT11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BU11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BV11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BW11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BX11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="16.05" customHeight="1" s="4">
       <c r="A12" s="3" t="inlineStr">
@@ -2684,6 +4202,171 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="AR12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AS12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AT12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AU12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AV12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AW12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AX12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AY12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AZ12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BA12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BB12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BC12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BD12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BE12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BF12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BG12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BH12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BI12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BJ12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BK12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BL12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BM12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BN12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BO12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BP12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BQ12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BR12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BS12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BT12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BU12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BV12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BW12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BX12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="13" ht="16.05" customHeight="1" s="4">
       <c r="A13" s="3" t="inlineStr">
@@ -2899,6 +4582,171 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="AR13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AS13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AT13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AU13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AV13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AW13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AX13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AY13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AZ13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BA13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BB13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BC13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BD13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BE13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BF13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BG13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BH13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BI13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BJ13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BK13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BL13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BM13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BN13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BO13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BP13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BQ13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BR13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BS13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BT13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BU13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BV13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BW13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BX13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="16.05" customHeight="1" s="4">
       <c r="A14" s="5" t="inlineStr">
@@ -3114,6 +4962,171 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="AR14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AS14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AT14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AU14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AV14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AW14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AX14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AY14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AZ14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BA14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BB14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BC14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BD14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BE14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BF14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BG14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BH14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BI14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BJ14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BK14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BL14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BM14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BN14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BO14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BP14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BQ14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BR14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BS14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BT14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BU14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BV14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BW14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BX14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="16.05" customHeight="1" s="4">
       <c r="A15" s="5" t="inlineStr">
@@ -3325,6 +5338,171 @@
         </is>
       </c>
       <c r="AQ15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AR15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AS15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AT15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AU15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AV15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AW15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AX15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AY15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AZ15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BA15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BB15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BC15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BD15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BE15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BF15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BG15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BH15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BI15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BJ15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BK15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BL15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BM15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BN15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BO15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BP15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BQ15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BR15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BS15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BT15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BU15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BV15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BW15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BX15" s="3" t="inlineStr">
         <is>
           <t>group1</t>
         </is>

</xml_diff>

<commit_message>
Ajout d'un fichier utils.py pour les sous-fonctions + rajout d'un fichier test.xlsx non corrompu
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_column_set_answer.xlsx
+++ b/fichiers_xls/test_column_set_answer.xlsx
@@ -462,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:BX15"/>
+  <dimension ref="A1:BY15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -865,6 +865,11 @@
           <t>group3</t>
         </is>
       </c>
+      <c r="BY2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="16.05" customHeight="1" s="4">
       <c r="A3" s="3" t="inlineStr">
@@ -1245,6 +1250,11 @@
           <t>group1</t>
         </is>
       </c>
+      <c r="BY3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="16.05" customHeight="1" s="4">
       <c r="A4" s="3" t="inlineStr">
@@ -1625,6 +1635,11 @@
           <t>group3</t>
         </is>
       </c>
+      <c r="BY4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="16.05" customHeight="1" s="4">
       <c r="A5" s="3" t="inlineStr">
@@ -2005,6 +2020,11 @@
           <t>group3</t>
         </is>
       </c>
+      <c r="BY5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="16.05" customHeight="1" s="4">
       <c r="A6" s="3" t="inlineStr">
@@ -2385,6 +2405,11 @@
           <t>group1</t>
         </is>
       </c>
+      <c r="BY6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="16.05" customHeight="1" s="4">
       <c r="A7" s="3" t="inlineStr">
@@ -2765,6 +2790,11 @@
           <t>group1</t>
         </is>
       </c>
+      <c r="BY7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="16.05" customHeight="1" s="4">
       <c r="A8" s="3" t="inlineStr">
@@ -3145,6 +3175,11 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="BY8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="16.05" customHeight="1" s="4">
       <c r="A9" s="3" t="inlineStr">
@@ -3521,6 +3556,11 @@
         </is>
       </c>
       <c r="BX9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BY9" s="3" t="inlineStr">
         <is>
           <t>group2</t>
         </is>
@@ -3607,6 +3647,7 @@
       <c r="BV10" s="3" t="inlineStr"/>
       <c r="BW10" s="3" t="inlineStr"/>
       <c r="BX10" s="3" t="inlineStr"/>
+      <c r="BY10" s="3" t="inlineStr"/>
     </row>
     <row r="11" ht="16.05" customHeight="1" s="4">
       <c r="A11" s="3" t="inlineStr">
@@ -3987,6 +4028,11 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="BY11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="16.05" customHeight="1" s="4">
       <c r="A12" s="3" t="inlineStr">
@@ -4367,6 +4413,11 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="BY12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="13" ht="16.05" customHeight="1" s="4">
       <c r="A13" s="3" t="inlineStr">
@@ -4747,6 +4798,11 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="BY13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="16.05" customHeight="1" s="4">
       <c r="A14" s="5" t="inlineStr">
@@ -5127,6 +5183,11 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="BY14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="16.05" customHeight="1" s="4">
       <c r="A15" s="5" t="inlineStr">
@@ -5503,6 +5564,11 @@
         </is>
       </c>
       <c r="BX15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BY15" s="3" t="inlineStr">
         <is>
           <t>group1</t>
         </is>

</xml_diff>

<commit_message>
Déplacement des fonctions annexes dans utils.py
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_column_set_answer.xlsx
+++ b/fichiers_xls/test_column_set_answer.xlsx
@@ -462,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:BY15"/>
+  <dimension ref="A1:CL15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -870,6 +870,71 @@
           <t>group3</t>
         </is>
       </c>
+      <c r="BZ2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CA2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CB2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CC2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CD2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CE2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CF2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CG2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CH2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CI2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CJ2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CK2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CL2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="16.05" customHeight="1" s="4">
       <c r="A3" s="3" t="inlineStr">
@@ -1255,6 +1320,71 @@
           <t>group1</t>
         </is>
       </c>
+      <c r="BZ3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CA3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CB3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CC3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CD3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CE3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CF3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CG3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CH3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CI3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CJ3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CK3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CL3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="16.05" customHeight="1" s="4">
       <c r="A4" s="3" t="inlineStr">
@@ -1640,6 +1770,71 @@
           <t>group3</t>
         </is>
       </c>
+      <c r="BZ4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CA4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CB4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CC4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CD4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CE4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CF4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CG4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CH4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CI4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CJ4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CK4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CL4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="16.05" customHeight="1" s="4">
       <c r="A5" s="3" t="inlineStr">
@@ -2025,6 +2220,71 @@
           <t>group3</t>
         </is>
       </c>
+      <c r="BZ5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CA5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CB5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CC5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CD5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CE5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CF5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CG5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CH5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CI5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CJ5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CK5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CL5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="16.05" customHeight="1" s="4">
       <c r="A6" s="3" t="inlineStr">
@@ -2410,6 +2670,71 @@
           <t>group1</t>
         </is>
       </c>
+      <c r="BZ6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CA6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CB6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CC6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CD6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CE6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CF6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CG6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CH6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CI6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CJ6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CK6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CL6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="16.05" customHeight="1" s="4">
       <c r="A7" s="3" t="inlineStr">
@@ -2795,6 +3120,71 @@
           <t>group1</t>
         </is>
       </c>
+      <c r="BZ7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CA7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CB7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CC7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CD7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CE7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CF7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CG7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CH7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CI7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CJ7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CK7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CL7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="16.05" customHeight="1" s="4">
       <c r="A8" s="3" t="inlineStr">
@@ -3180,6 +3570,71 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="BZ8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CA8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CB8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CC8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CD8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CE8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CF8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CG8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CH8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CI8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CJ8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CK8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CL8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="16.05" customHeight="1" s="4">
       <c r="A9" s="3" t="inlineStr">
@@ -3561,6 +4016,71 @@
         </is>
       </c>
       <c r="BY9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BZ9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CA9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CB9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CC9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CD9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CE9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CF9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CG9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CH9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CI9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CJ9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CK9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CL9" s="3" t="inlineStr">
         <is>
           <t>group2</t>
         </is>
@@ -3648,6 +4168,19 @@
       <c r="BW10" s="3" t="inlineStr"/>
       <c r="BX10" s="3" t="inlineStr"/>
       <c r="BY10" s="3" t="inlineStr"/>
+      <c r="BZ10" s="3" t="inlineStr"/>
+      <c r="CA10" s="3" t="inlineStr"/>
+      <c r="CB10" s="3" t="inlineStr"/>
+      <c r="CC10" s="3" t="inlineStr"/>
+      <c r="CD10" s="3" t="inlineStr"/>
+      <c r="CE10" s="3" t="inlineStr"/>
+      <c r="CF10" s="3" t="inlineStr"/>
+      <c r="CG10" s="3" t="inlineStr"/>
+      <c r="CH10" s="3" t="inlineStr"/>
+      <c r="CI10" s="3" t="inlineStr"/>
+      <c r="CJ10" s="3" t="inlineStr"/>
+      <c r="CK10" s="3" t="inlineStr"/>
+      <c r="CL10" s="3" t="inlineStr"/>
     </row>
     <row r="11" ht="16.05" customHeight="1" s="4">
       <c r="A11" s="3" t="inlineStr">
@@ -4033,6 +4566,71 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="BZ11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CA11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CB11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CC11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CD11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CE11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CF11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CG11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CH11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CI11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CJ11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CK11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CL11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="16.05" customHeight="1" s="4">
       <c r="A12" s="3" t="inlineStr">
@@ -4418,6 +5016,71 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="BZ12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CA12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CB12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CC12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CD12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CE12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CF12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CG12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CH12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CI12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CJ12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CK12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CL12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="13" ht="16.05" customHeight="1" s="4">
       <c r="A13" s="3" t="inlineStr">
@@ -4803,6 +5466,71 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="BZ13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CA13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CB13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CC13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CD13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CE13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CF13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CG13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CH13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CI13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CJ13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CK13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CL13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="16.05" customHeight="1" s="4">
       <c r="A14" s="5" t="inlineStr">
@@ -5188,6 +5916,71 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="BZ14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CA14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CB14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CC14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CD14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CE14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CF14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CG14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CH14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CI14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CJ14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CK14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CL14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="16.05" customHeight="1" s="4">
       <c r="A15" s="5" t="inlineStr">
@@ -5569,6 +6362,71 @@
         </is>
       </c>
       <c r="BY15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BZ15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CA15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CB15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CC15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CD15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CE15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CF15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CG15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CH15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CI15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CJ15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CK15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CL15" s="3" t="inlineStr">
         <is>
           <t>group1</t>
         </is>

</xml_diff>

<commit_message>
Ajout de  extract_column_from_all_sheets et d'un test.
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_column_set_answer.xlsx
+++ b/fichiers_xls/test_column_set_answer.xlsx
@@ -462,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:CL15"/>
+  <dimension ref="A1:DG15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -935,6 +935,111 @@
           <t>group3</t>
         </is>
       </c>
+      <c r="CM2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CN2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CO2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CP2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CQ2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CR2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CS2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CT2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CU2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CV2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CW2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CX2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CY2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CZ2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DA2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DB2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DC2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DD2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DE2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DF2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DG2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="16.05" customHeight="1" s="4">
       <c r="A3" s="3" t="inlineStr">
@@ -1385,6 +1490,111 @@
           <t>group1</t>
         </is>
       </c>
+      <c r="CM3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CN3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CO3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CP3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CQ3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CR3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CS3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CT3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CU3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CV3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CW3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CX3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CY3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CZ3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DA3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DB3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DC3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DD3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DE3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DF3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DG3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="16.05" customHeight="1" s="4">
       <c r="A4" s="3" t="inlineStr">
@@ -1835,6 +2045,111 @@
           <t>group3</t>
         </is>
       </c>
+      <c r="CM4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CN4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CO4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CP4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CQ4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CR4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CS4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CT4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CU4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CV4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CW4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CX4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CY4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CZ4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DA4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DB4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DC4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DD4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DE4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DF4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DG4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="16.05" customHeight="1" s="4">
       <c r="A5" s="3" t="inlineStr">
@@ -2285,6 +2600,111 @@
           <t>group3</t>
         </is>
       </c>
+      <c r="CM5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CN5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CO5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CP5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CQ5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CR5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CS5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CT5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CU5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CV5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CW5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CX5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CY5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CZ5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DA5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DB5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DC5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DD5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DE5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DF5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="DG5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="16.05" customHeight="1" s="4">
       <c r="A6" s="3" t="inlineStr">
@@ -2735,6 +3155,111 @@
           <t>group1</t>
         </is>
       </c>
+      <c r="CM6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CN6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CO6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CP6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CQ6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CR6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CS6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CT6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CU6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CV6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CW6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CX6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CY6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CZ6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DA6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DB6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DC6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DD6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DE6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DF6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DG6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="16.05" customHeight="1" s="4">
       <c r="A7" s="3" t="inlineStr">
@@ -3185,6 +3710,111 @@
           <t>group1</t>
         </is>
       </c>
+      <c r="CM7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CN7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CO7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CP7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CQ7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CR7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CS7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CT7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CU7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CV7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CW7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CX7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CY7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CZ7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DA7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DB7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DC7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DD7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DE7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DF7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DG7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="16.05" customHeight="1" s="4">
       <c r="A8" s="3" t="inlineStr">
@@ -3635,6 +4265,111 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="CM8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CN8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CO8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CP8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CQ8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CR8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CS8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CT8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CU8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CV8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CW8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CX8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CY8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CZ8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DA8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DB8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DC8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DD8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DE8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DF8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DG8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="16.05" customHeight="1" s="4">
       <c r="A9" s="3" t="inlineStr">
@@ -4081,6 +4816,111 @@
         </is>
       </c>
       <c r="CL9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CM9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CN9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CO9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CP9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CQ9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CR9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CS9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CT9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CU9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CV9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CW9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CX9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CY9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CZ9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DA9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DB9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DC9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DD9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DE9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DF9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DG9" s="3" t="inlineStr">
         <is>
           <t>group2</t>
         </is>
@@ -4181,6 +5021,27 @@
       <c r="CJ10" s="3" t="inlineStr"/>
       <c r="CK10" s="3" t="inlineStr"/>
       <c r="CL10" s="3" t="inlineStr"/>
+      <c r="CM10" s="3" t="inlineStr"/>
+      <c r="CN10" s="3" t="inlineStr"/>
+      <c r="CO10" s="3" t="inlineStr"/>
+      <c r="CP10" s="3" t="inlineStr"/>
+      <c r="CQ10" s="3" t="inlineStr"/>
+      <c r="CR10" s="3" t="inlineStr"/>
+      <c r="CS10" s="3" t="inlineStr"/>
+      <c r="CT10" s="3" t="inlineStr"/>
+      <c r="CU10" s="3" t="inlineStr"/>
+      <c r="CV10" s="3" t="inlineStr"/>
+      <c r="CW10" s="3" t="inlineStr"/>
+      <c r="CX10" s="3" t="inlineStr"/>
+      <c r="CY10" s="3" t="inlineStr"/>
+      <c r="CZ10" s="3" t="inlineStr"/>
+      <c r="DA10" s="3" t="inlineStr"/>
+      <c r="DB10" s="3" t="inlineStr"/>
+      <c r="DC10" s="3" t="inlineStr"/>
+      <c r="DD10" s="3" t="inlineStr"/>
+      <c r="DE10" s="3" t="inlineStr"/>
+      <c r="DF10" s="3" t="inlineStr"/>
+      <c r="DG10" s="3" t="inlineStr"/>
     </row>
     <row r="11" ht="16.05" customHeight="1" s="4">
       <c r="A11" s="3" t="inlineStr">
@@ -4631,6 +5492,111 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="CM11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CN11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CO11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CP11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CQ11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CR11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CS11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CT11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CU11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CV11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CW11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CX11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CY11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CZ11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DA11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DB11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DC11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DD11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DE11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DF11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DG11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="16.05" customHeight="1" s="4">
       <c r="A12" s="3" t="inlineStr">
@@ -5081,6 +6047,111 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="CM12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CN12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CO12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CP12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CQ12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CR12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CS12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CT12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CU12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CV12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CW12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CX12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CY12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CZ12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DA12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DB12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DC12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DD12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DE12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DF12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DG12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="13" ht="16.05" customHeight="1" s="4">
       <c r="A13" s="3" t="inlineStr">
@@ -5531,6 +6602,111 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="CM13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CN13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CO13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CP13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CQ13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CR13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CS13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CT13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CU13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CV13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CW13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CX13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CY13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CZ13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DA13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DB13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DC13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DD13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DE13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DF13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DG13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="16.05" customHeight="1" s="4">
       <c r="A14" s="5" t="inlineStr">
@@ -5981,6 +7157,111 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="CM14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CN14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CO14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CP14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CQ14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CR14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CS14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CT14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CU14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CV14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CW14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CX14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CY14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CZ14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DA14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DB14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DC14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DD14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DE14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DF14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="DG14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="16.05" customHeight="1" s="4">
       <c r="A15" s="5" t="inlineStr">
@@ -6427,6 +7708,111 @@
         </is>
       </c>
       <c r="CL15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CM15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CN15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CO15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CP15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CQ15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CR15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CS15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CT15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CU15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CV15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CW15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CX15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CY15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CZ15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DA15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DB15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DC15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DD15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DE15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DF15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="DG15" s="3" t="inlineStr">
         <is>
           <t>group1</t>
         </is>

</xml_diff>

<commit_message>
Ajout de delete doublons
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_column_set_answer.xlsx
+++ b/fichiers_xls/test_column_set_answer.xlsx
@@ -462,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:EO15"/>
+  <dimension ref="A1:FJ15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -1210,6 +1210,111 @@
           <t>group3</t>
         </is>
       </c>
+      <c r="EP2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EQ2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="ER2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="ES2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="ET2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EU2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EV2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EW2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EX2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EY2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EZ2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FA2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FB2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FC2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FD2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FE2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FF2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FG2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FH2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FI2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FJ2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="16.05" customHeight="1" s="4">
       <c r="A3" s="3" t="inlineStr">
@@ -1935,6 +2040,111 @@
           <t>group1</t>
         </is>
       </c>
+      <c r="EP3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EQ3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="ER3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="ES3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="ET3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EU3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EV3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EW3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EX3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EY3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EZ3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FA3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FB3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FC3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FD3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FE3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FF3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FG3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FH3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FI3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FJ3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="16.05" customHeight="1" s="4">
       <c r="A4" s="3" t="inlineStr">
@@ -2660,6 +2870,111 @@
           <t>group3</t>
         </is>
       </c>
+      <c r="EP4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EQ4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="ER4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="ES4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="ET4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EU4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EV4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EW4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EX4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EY4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EZ4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FA4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FB4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FC4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FD4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FE4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FF4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FG4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FH4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FI4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FJ4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="16.05" customHeight="1" s="4">
       <c r="A5" s="3" t="inlineStr">
@@ -3385,6 +3700,111 @@
           <t>group3</t>
         </is>
       </c>
+      <c r="EP5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EQ5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="ER5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="ES5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="ET5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EU5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EV5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EW5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EX5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EY5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="EZ5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FA5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FB5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FC5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FD5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FE5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FF5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FG5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FH5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FI5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="FJ5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="16.05" customHeight="1" s="4">
       <c r="A6" s="3" t="inlineStr">
@@ -4110,6 +4530,111 @@
           <t>group1</t>
         </is>
       </c>
+      <c r="EP6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EQ6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="ER6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="ES6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="ET6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EU6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EV6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EW6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EX6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EY6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EZ6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FA6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FB6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FC6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FD6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FE6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FF6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FG6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FH6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FI6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FJ6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="16.05" customHeight="1" s="4">
       <c r="A7" s="3" t="inlineStr">
@@ -4835,6 +5360,111 @@
           <t>group1</t>
         </is>
       </c>
+      <c r="EP7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EQ7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="ER7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="ES7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="ET7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EU7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EV7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EW7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EX7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EY7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EZ7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FA7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FB7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FC7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FD7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FE7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FF7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FG7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FH7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FI7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FJ7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="16.05" customHeight="1" s="4">
       <c r="A8" s="3" t="inlineStr">
@@ -5560,6 +6190,111 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="EP8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EQ8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="ER8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="ES8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="ET8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EU8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EV8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EW8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EX8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EY8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EZ8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FA8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FB8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FC8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FD8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FE8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FF8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FG8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FH8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FI8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FJ8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="16.05" customHeight="1" s="4">
       <c r="A9" s="3" t="inlineStr">
@@ -6281,6 +7016,111 @@
         </is>
       </c>
       <c r="EO9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EP9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EQ9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="ER9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="ES9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="ET9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EU9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EV9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EW9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EX9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EY9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EZ9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FA9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FB9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FC9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FD9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FE9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FF9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FG9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FH9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FI9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FJ9" s="3" t="inlineStr">
         <is>
           <t>group2</t>
         </is>
@@ -6436,6 +7276,27 @@
       <c r="EM10" s="3" t="inlineStr"/>
       <c r="EN10" s="3" t="inlineStr"/>
       <c r="EO10" s="3" t="inlineStr"/>
+      <c r="EP10" s="3" t="inlineStr"/>
+      <c r="EQ10" s="3" t="inlineStr"/>
+      <c r="ER10" s="3" t="inlineStr"/>
+      <c r="ES10" s="3" t="inlineStr"/>
+      <c r="ET10" s="3" t="inlineStr"/>
+      <c r="EU10" s="3" t="inlineStr"/>
+      <c r="EV10" s="3" t="inlineStr"/>
+      <c r="EW10" s="3" t="inlineStr"/>
+      <c r="EX10" s="3" t="inlineStr"/>
+      <c r="EY10" s="3" t="inlineStr"/>
+      <c r="EZ10" s="3" t="inlineStr"/>
+      <c r="FA10" s="3" t="inlineStr"/>
+      <c r="FB10" s="3" t="inlineStr"/>
+      <c r="FC10" s="3" t="inlineStr"/>
+      <c r="FD10" s="3" t="inlineStr"/>
+      <c r="FE10" s="3" t="inlineStr"/>
+      <c r="FF10" s="3" t="inlineStr"/>
+      <c r="FG10" s="3" t="inlineStr"/>
+      <c r="FH10" s="3" t="inlineStr"/>
+      <c r="FI10" s="3" t="inlineStr"/>
+      <c r="FJ10" s="3" t="inlineStr"/>
     </row>
     <row r="11" ht="16.05" customHeight="1" s="4">
       <c r="A11" s="3" t="inlineStr">
@@ -7161,6 +8022,111 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="EP11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EQ11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="ER11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="ES11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="ET11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EU11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EV11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EW11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EX11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EY11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EZ11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FA11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FB11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FC11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FD11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FE11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FF11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FG11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FH11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FI11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FJ11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="16.05" customHeight="1" s="4">
       <c r="A12" s="3" t="inlineStr">
@@ -7886,6 +8852,111 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="EP12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EQ12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="ER12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="ES12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="ET12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EU12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EV12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EW12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EX12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EY12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EZ12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FA12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FB12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FC12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FD12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FE12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FF12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FG12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FH12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FI12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FJ12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="13" ht="16.05" customHeight="1" s="4">
       <c r="A13" s="3" t="inlineStr">
@@ -8611,6 +9682,111 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="EP13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EQ13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="ER13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="ES13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="ET13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EU13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EV13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EW13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EX13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EY13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EZ13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FA13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FB13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FC13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FD13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FE13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FF13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FG13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FH13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FI13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FJ13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="16.05" customHeight="1" s="4">
       <c r="A14" s="5" t="inlineStr">
@@ -9336,6 +10512,111 @@
           <t>group2</t>
         </is>
       </c>
+      <c r="EP14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EQ14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="ER14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="ES14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="ET14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EU14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EV14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EW14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EX14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EY14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="EZ14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FA14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FB14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FC14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FD14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FE14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FF14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FG14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FH14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FI14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="FJ14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="16.05" customHeight="1" s="4">
       <c r="A15" s="5" t="inlineStr">
@@ -10057,6 +11338,111 @@
         </is>
       </c>
       <c r="EO15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EP15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EQ15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="ER15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="ES15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="ET15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EU15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EV15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EW15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EX15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EY15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="EZ15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FA15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FB15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FC15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FD15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FE15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FF15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FG15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FH15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FI15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="FJ15" s="3" t="inlineStr">
         <is>
           <t>group1</t>
         </is>

</xml_diff>

<commit_message>
feat(sheet) Add the sheet function gather_multiple_answers
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_column_set_answer.xlsx
+++ b/fichiers_xls/test_column_set_answer.xlsx
@@ -462,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:X15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -507,6 +507,101 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="H2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="I2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="J2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="K2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="L2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="M2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="N2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="O2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="P2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="Q2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="R2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="S2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="T2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="U2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="V2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="W2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="X2" s="3" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -532,6 +627,101 @@
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="K3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="L3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="M3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="N3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="O3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="P3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="Q3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="R3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="S3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="T3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="U3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="V3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="W3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="X3" s="3" t="inlineStr">
+        <is>
           <t>9</t>
         </is>
       </c>
@@ -557,6 +747,101 @@
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="H4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="I4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="J4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="K4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="L4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="M4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="N4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="O4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="P4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="Q4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="R4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="S4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="T4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="U4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="V4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="W4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="X4" s="3" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
@@ -582,6 +867,101 @@
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="I5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="J5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="K5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="L5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="M5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="N5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="O5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="P5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="Q5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="R5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="S5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="T5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="U5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="V5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="W5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="X5" s="3" t="inlineStr">
+        <is>
           <t>10</t>
         </is>
       </c>
@@ -605,7 +985,102 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="E6" s="3" t="inlineStr"/>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="I6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="J6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="K6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="L6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="M6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="N6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="O6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="P6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="Q6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="R6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="S6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="T6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="U6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="V6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="W6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="X6" s="3" t="inlineStr"/>
     </row>
     <row r="7" ht="16.05" customHeight="1" s="4">
       <c r="A7" s="3" t="inlineStr">
@@ -626,7 +1101,102 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="E7" s="3" t="inlineStr"/>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="I7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="J7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="K7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="L7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="M7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="N7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="O7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="P7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="Q7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="R7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="S7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="T7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="U7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="V7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="W7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="X7" s="3" t="inlineStr"/>
     </row>
     <row r="8" ht="16.05" customHeight="1" s="4">
       <c r="A8" s="3" t="inlineStr">
@@ -647,7 +1217,102 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="E8" s="3" t="inlineStr"/>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="I8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="J8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="K8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="L8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="M8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="N8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="O8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="P8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="Q8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="R8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="S8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="T8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="U8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="V8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="W8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="X8" s="3" t="inlineStr"/>
     </row>
     <row r="9" ht="16.05" customHeight="1" s="4">
       <c r="A9" s="3" t="inlineStr">
@@ -668,7 +1333,102 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="E9" s="3" t="inlineStr"/>
+      <c r="E9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="G9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="J9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="L9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="M9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="N9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="O9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="P9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="Q9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="R9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="S9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="T9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="U9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="V9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="W9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="X9" s="3" t="inlineStr"/>
     </row>
     <row r="10" ht="16.05" customHeight="1" s="4">
       <c r="A10" s="3" t="inlineStr">
@@ -680,6 +1440,25 @@
       <c r="C10" t="inlineStr"/>
       <c r="D10" s="3" t="inlineStr"/>
       <c r="E10" s="3" t="inlineStr"/>
+      <c r="F10" s="3" t="inlineStr"/>
+      <c r="G10" s="3" t="inlineStr"/>
+      <c r="H10" s="3" t="inlineStr"/>
+      <c r="I10" s="3" t="inlineStr"/>
+      <c r="J10" s="3" t="inlineStr"/>
+      <c r="K10" s="3" t="inlineStr"/>
+      <c r="L10" s="3" t="inlineStr"/>
+      <c r="M10" s="3" t="inlineStr"/>
+      <c r="N10" s="3" t="inlineStr"/>
+      <c r="O10" s="3" t="inlineStr"/>
+      <c r="P10" s="3" t="inlineStr"/>
+      <c r="Q10" s="3" t="inlineStr"/>
+      <c r="R10" s="3" t="inlineStr"/>
+      <c r="S10" s="3" t="inlineStr"/>
+      <c r="T10" s="3" t="inlineStr"/>
+      <c r="U10" s="3" t="inlineStr"/>
+      <c r="V10" s="3" t="inlineStr"/>
+      <c r="W10" s="3" t="inlineStr"/>
+      <c r="X10" s="3" t="inlineStr"/>
     </row>
     <row r="11" ht="16.05" customHeight="1" s="4">
       <c r="A11" s="3" t="inlineStr">
@@ -700,7 +1479,102 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr"/>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="G11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="J11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="K11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="L11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="N11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="O11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="P11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="Q11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="R11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="S11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="T11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="U11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="V11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="W11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="X11" s="3" t="inlineStr"/>
     </row>
     <row r="12" ht="16.05" customHeight="1" s="4">
       <c r="A12" s="3" t="inlineStr">
@@ -721,7 +1595,102 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="E12" s="3" t="inlineStr"/>
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="G12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="L12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="N12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="O12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="P12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="Q12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="R12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="S12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="T12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="U12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="V12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="W12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="X12" s="3" t="inlineStr"/>
     </row>
     <row r="13" ht="16.05" customHeight="1" s="4">
       <c r="A13" s="3" t="inlineStr">
@@ -742,7 +1711,102 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="E13" s="3" t="inlineStr"/>
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="G13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="K13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="L13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="N13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="O13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="P13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="Q13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="R13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="S13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="T13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="U13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="V13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="W13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="X13" s="3" t="inlineStr"/>
     </row>
     <row r="14" ht="16.05" customHeight="1" s="4">
       <c r="A14" s="5" t="inlineStr">
@@ -763,7 +1827,102 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="E14" s="3" t="inlineStr"/>
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="F14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="G14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="M14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="N14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="O14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="P14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="Q14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="R14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="S14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="T14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="U14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="V14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="W14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="X14" s="3" t="inlineStr"/>
     </row>
     <row r="15" ht="16.05" customHeight="1" s="4">
       <c r="A15" s="5" t="inlineStr">
@@ -784,7 +1943,102 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="E15" s="3" t="inlineStr"/>
+      <c r="E15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="M15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="N15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="O15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="P15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="Q15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="R15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="S15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="T15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="U15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="V15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="W15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="X15" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>

<commit_message>
feat(command) : Add some commands.
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_column_set_answer.xlsx
+++ b/fichiers_xls/test_column_set_answer.xlsx
@@ -462,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:X15"/>
+  <dimension ref="A1:AD15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -602,6 +602,36 @@
       </c>
       <c r="X2" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="Y2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="Z2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AA2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AB2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AC2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AD2" s="3" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -722,6 +752,36 @@
       </c>
       <c r="X3" s="3" t="inlineStr">
         <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="Y3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="Z3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AA3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AB3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AC3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AD3" s="3" t="inlineStr">
+        <is>
           <t>9</t>
         </is>
       </c>
@@ -842,6 +902,36 @@
       </c>
       <c r="X4" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="Y4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="Z4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AA4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AB4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AC4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AD4" s="3" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
@@ -962,6 +1052,36 @@
       </c>
       <c r="X5" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="Y5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="Z5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AA5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AB5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AC5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AD5" s="3" t="inlineStr">
+        <is>
           <t>10</t>
         </is>
       </c>
@@ -1080,7 +1200,37 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="X6" s="3" t="inlineStr"/>
+      <c r="X6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="Y6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="Z6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AA6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AB6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AC6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AD6" s="3" t="inlineStr"/>
     </row>
     <row r="7" ht="16.05" customHeight="1" s="4">
       <c r="A7" s="3" t="inlineStr">
@@ -1196,7 +1346,37 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="X7" s="3" t="inlineStr"/>
+      <c r="X7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="Y7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="Z7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AA7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AB7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AC7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AD7" s="3" t="inlineStr"/>
     </row>
     <row r="8" ht="16.05" customHeight="1" s="4">
       <c r="A8" s="3" t="inlineStr">
@@ -1312,7 +1492,37 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="X8" s="3" t="inlineStr"/>
+      <c r="X8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="Y8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="Z8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AA8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AB8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AC8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AD8" s="3" t="inlineStr"/>
     </row>
     <row r="9" ht="16.05" customHeight="1" s="4">
       <c r="A9" s="3" t="inlineStr">
@@ -1428,7 +1638,37 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="X9" s="3" t="inlineStr"/>
+      <c r="X9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="Y9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="Z9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AA9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AB9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AC9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AD9" s="3" t="inlineStr"/>
     </row>
     <row r="10" ht="16.05" customHeight="1" s="4">
       <c r="A10" s="3" t="inlineStr">
@@ -1459,6 +1699,12 @@
       <c r="V10" s="3" t="inlineStr"/>
       <c r="W10" s="3" t="inlineStr"/>
       <c r="X10" s="3" t="inlineStr"/>
+      <c r="Y10" s="3" t="inlineStr"/>
+      <c r="Z10" s="3" t="inlineStr"/>
+      <c r="AA10" s="3" t="inlineStr"/>
+      <c r="AB10" s="3" t="inlineStr"/>
+      <c r="AC10" s="3" t="inlineStr"/>
+      <c r="AD10" s="3" t="inlineStr"/>
     </row>
     <row r="11" ht="16.05" customHeight="1" s="4">
       <c r="A11" s="3" t="inlineStr">
@@ -1574,7 +1820,37 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="X11" s="3" t="inlineStr"/>
+      <c r="X11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="Y11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="Z11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AA11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AB11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AC11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AD11" s="3" t="inlineStr"/>
     </row>
     <row r="12" ht="16.05" customHeight="1" s="4">
       <c r="A12" s="3" t="inlineStr">
@@ -1690,7 +1966,37 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="X12" s="3" t="inlineStr"/>
+      <c r="X12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="Y12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="Z12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AA12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AB12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AC12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AD12" s="3" t="inlineStr"/>
     </row>
     <row r="13" ht="16.05" customHeight="1" s="4">
       <c r="A13" s="3" t="inlineStr">
@@ -1806,7 +2112,37 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="X13" s="3" t="inlineStr"/>
+      <c r="X13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="Y13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="Z13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AA13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AB13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AC13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AD13" s="3" t="inlineStr"/>
     </row>
     <row r="14" ht="16.05" customHeight="1" s="4">
       <c r="A14" s="5" t="inlineStr">
@@ -1922,7 +2258,37 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="X14" s="3" t="inlineStr"/>
+      <c r="X14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="Y14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="Z14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AA14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AB14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AC14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AD14" s="3" t="inlineStr"/>
     </row>
     <row r="15" ht="16.05" customHeight="1" s="4">
       <c r="A15" s="5" t="inlineStr">
@@ -2038,7 +2404,37 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="X15" s="3" t="inlineStr"/>
+      <c r="X15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="Y15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="Z15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AA15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AB15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AC15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AD15" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>

<commit_message>
refactor(module,command) : add a possibility for some methods for the user writing commands to overwrite the writing column rather than inserting a new column.
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_column_set_answer.xlsx
+++ b/fichiers_xls/test_column_set_answer.xlsx
@@ -462,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:AI15"/>
+  <dimension ref="A1:AJ15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -657,6 +657,11 @@
       </c>
       <c r="AI2" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AJ2" s="3" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -832,6 +837,11 @@
       </c>
       <c r="AI3" s="3" t="inlineStr">
         <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AJ3" s="3" t="inlineStr">
+        <is>
           <t>9</t>
         </is>
       </c>
@@ -1007,6 +1017,11 @@
       </c>
       <c r="AI4" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AJ4" s="3" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
@@ -1182,6 +1197,11 @@
       </c>
       <c r="AI5" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AJ5" s="3" t="inlineStr">
+        <is>
           <t>10</t>
         </is>
       </c>
@@ -1355,7 +1375,12 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="AI6" s="3" t="inlineStr"/>
+      <c r="AI6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AJ6" s="3" t="inlineStr"/>
     </row>
     <row r="7" ht="16.05" customHeight="1" s="4">
       <c r="A7" s="3" t="inlineStr">
@@ -1526,7 +1551,12 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="AI7" s="3" t="inlineStr"/>
+      <c r="AI7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AJ7" s="3" t="inlineStr"/>
     </row>
     <row r="8" ht="16.05" customHeight="1" s="4">
       <c r="A8" s="3" t="inlineStr">
@@ -1697,7 +1727,12 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="AI8" s="3" t="inlineStr"/>
+      <c r="AI8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AJ8" s="3" t="inlineStr"/>
     </row>
     <row r="9" ht="16.05" customHeight="1" s="4">
       <c r="A9" s="3" t="inlineStr">
@@ -1868,7 +1903,12 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="AI9" s="3" t="inlineStr"/>
+      <c r="AI9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AJ9" s="3" t="inlineStr"/>
     </row>
     <row r="10" ht="16.05" customHeight="1" s="4">
       <c r="A10" s="3" t="inlineStr">
@@ -1910,6 +1950,7 @@
       <c r="AG10" s="3" t="inlineStr"/>
       <c r="AH10" s="3" t="inlineStr"/>
       <c r="AI10" s="3" t="inlineStr"/>
+      <c r="AJ10" s="3" t="inlineStr"/>
     </row>
     <row r="11" ht="16.05" customHeight="1" s="4">
       <c r="A11" s="3" t="inlineStr">
@@ -2080,7 +2121,12 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="AI11" s="3" t="inlineStr"/>
+      <c r="AI11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AJ11" s="3" t="inlineStr"/>
     </row>
     <row r="12" ht="16.05" customHeight="1" s="4">
       <c r="A12" s="3" t="inlineStr">
@@ -2251,7 +2297,12 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="AI12" s="3" t="inlineStr"/>
+      <c r="AI12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AJ12" s="3" t="inlineStr"/>
     </row>
     <row r="13" ht="16.05" customHeight="1" s="4">
       <c r="A13" s="3" t="inlineStr">
@@ -2422,7 +2473,12 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="AI13" s="3" t="inlineStr"/>
+      <c r="AI13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AJ13" s="3" t="inlineStr"/>
     </row>
     <row r="14" ht="16.05" customHeight="1" s="4">
       <c r="A14" s="5" t="inlineStr">
@@ -2593,7 +2649,12 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="AI14" s="3" t="inlineStr"/>
+      <c r="AI14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AJ14" s="3" t="inlineStr"/>
     </row>
     <row r="15" ht="16.05" customHeight="1" s="4">
       <c r="A15" s="5" t="inlineStr">
@@ -2764,7 +2825,12 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="AI15" s="3" t="inlineStr"/>
+      <c r="AI15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AJ15" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>

<commit_message>
feat(module) : add a function gather_columns_in_one.
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_column_set_answer.xlsx
+++ b/fichiers_xls/test_column_set_answer.xlsx
@@ -462,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:AJ15"/>
+  <dimension ref="A1:BC15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -662,6 +662,101 @@
       </c>
       <c r="AJ2" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AK2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AL2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AM2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AN2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AO2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AP2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AQ2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AR2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AS2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AT2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AU2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AV2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AW2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AX2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AY2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AZ2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BA2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BB2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BC2" s="3" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -842,6 +937,101 @@
       </c>
       <c r="AJ3" s="3" t="inlineStr">
         <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AK3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AL3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AM3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AN3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AO3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AP3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AQ3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AR3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AS3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AT3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AU3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AV3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AW3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AX3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AY3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AZ3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BA3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BB3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BC3" s="3" t="inlineStr">
+        <is>
           <t>9</t>
         </is>
       </c>
@@ -1022,6 +1212,101 @@
       </c>
       <c r="AJ4" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AK4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AL4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AM4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AN4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AO4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AP4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AQ4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AR4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AS4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AT4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AU4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AV4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AW4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AX4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AY4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AZ4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BA4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BB4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BC4" s="3" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
@@ -1202,6 +1487,101 @@
       </c>
       <c r="AJ5" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AK5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AL5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AM5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AN5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AO5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AP5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AQ5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AR5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AS5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AT5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AU5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AV5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AW5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AX5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AY5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="AZ5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BA5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BB5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BC5" s="3" t="inlineStr">
+        <is>
           <t>10</t>
         </is>
       </c>
@@ -1380,7 +1760,102 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="AJ6" s="3" t="inlineStr"/>
+      <c r="AJ6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AK6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AL6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AM6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AN6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AO6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AP6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AQ6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AR6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AS6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AT6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AU6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AV6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AW6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AX6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AY6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AZ6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BA6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BB6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BC6" s="3" t="inlineStr"/>
     </row>
     <row r="7" ht="16.05" customHeight="1" s="4">
       <c r="A7" s="3" t="inlineStr">
@@ -1556,7 +2031,102 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="AJ7" s="3" t="inlineStr"/>
+      <c r="AJ7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AK7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AL7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AM7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AN7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AO7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AP7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AQ7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AR7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AS7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AT7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AU7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AV7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AW7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AX7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AY7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AZ7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BA7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BB7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BC7" s="3" t="inlineStr"/>
     </row>
     <row r="8" ht="16.05" customHeight="1" s="4">
       <c r="A8" s="3" t="inlineStr">
@@ -1732,7 +2302,102 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="AJ8" s="3" t="inlineStr"/>
+      <c r="AJ8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AK8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AL8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AM8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AN8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AO8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AP8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AQ8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AR8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AS8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AT8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AU8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AV8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AW8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AX8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AY8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AZ8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BA8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BB8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BC8" s="3" t="inlineStr"/>
     </row>
     <row r="9" ht="16.05" customHeight="1" s="4">
       <c r="A9" s="3" t="inlineStr">
@@ -1908,7 +2573,102 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="AJ9" s="3" t="inlineStr"/>
+      <c r="AJ9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AK9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AL9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AM9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AN9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AO9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AP9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AQ9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AR9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AS9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AT9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AU9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AV9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AW9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AX9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AY9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AZ9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BA9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BB9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BC9" s="3" t="inlineStr"/>
     </row>
     <row r="10" ht="16.05" customHeight="1" s="4">
       <c r="A10" s="3" t="inlineStr">
@@ -1951,6 +2711,25 @@
       <c r="AH10" s="3" t="inlineStr"/>
       <c r="AI10" s="3" t="inlineStr"/>
       <c r="AJ10" s="3" t="inlineStr"/>
+      <c r="AK10" s="3" t="inlineStr"/>
+      <c r="AL10" s="3" t="inlineStr"/>
+      <c r="AM10" s="3" t="inlineStr"/>
+      <c r="AN10" s="3" t="inlineStr"/>
+      <c r="AO10" s="3" t="inlineStr"/>
+      <c r="AP10" s="3" t="inlineStr"/>
+      <c r="AQ10" s="3" t="inlineStr"/>
+      <c r="AR10" s="3" t="inlineStr"/>
+      <c r="AS10" s="3" t="inlineStr"/>
+      <c r="AT10" s="3" t="inlineStr"/>
+      <c r="AU10" s="3" t="inlineStr"/>
+      <c r="AV10" s="3" t="inlineStr"/>
+      <c r="AW10" s="3" t="inlineStr"/>
+      <c r="AX10" s="3" t="inlineStr"/>
+      <c r="AY10" s="3" t="inlineStr"/>
+      <c r="AZ10" s="3" t="inlineStr"/>
+      <c r="BA10" s="3" t="inlineStr"/>
+      <c r="BB10" s="3" t="inlineStr"/>
+      <c r="BC10" s="3" t="inlineStr"/>
     </row>
     <row r="11" ht="16.05" customHeight="1" s="4">
       <c r="A11" s="3" t="inlineStr">
@@ -2126,7 +2905,102 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="AJ11" s="3" t="inlineStr"/>
+      <c r="AJ11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AK11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AL11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AM11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AN11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AO11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AP11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AQ11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AR11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AS11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AT11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AU11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AV11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AW11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AX11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AY11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AZ11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BA11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BB11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BC11" s="3" t="inlineStr"/>
     </row>
     <row r="12" ht="16.05" customHeight="1" s="4">
       <c r="A12" s="3" t="inlineStr">
@@ -2302,7 +3176,102 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="AJ12" s="3" t="inlineStr"/>
+      <c r="AJ12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AK12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AL12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AM12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AN12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AO12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AP12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AQ12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AR12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AS12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AT12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AU12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AV12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AW12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AX12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AY12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AZ12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BA12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BB12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BC12" s="3" t="inlineStr"/>
     </row>
     <row r="13" ht="16.05" customHeight="1" s="4">
       <c r="A13" s="3" t="inlineStr">
@@ -2478,7 +3447,102 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="AJ13" s="3" t="inlineStr"/>
+      <c r="AJ13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AK13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AL13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AM13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AN13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AO13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AP13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AQ13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AR13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AS13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AT13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AU13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AV13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AW13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AX13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AY13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AZ13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BA13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BB13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BC13" s="3" t="inlineStr"/>
     </row>
     <row r="14" ht="16.05" customHeight="1" s="4">
       <c r="A14" s="5" t="inlineStr">
@@ -2654,7 +3718,102 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="AJ14" s="3" t="inlineStr"/>
+      <c r="AJ14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AK14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AL14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AM14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AN14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AO14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AP14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AQ14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AR14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AS14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AT14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AU14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AV14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AW14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AX14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AY14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="AZ14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BA14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BB14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BC14" s="3" t="inlineStr"/>
     </row>
     <row r="15" ht="16.05" customHeight="1" s="4">
       <c r="A15" s="5" t="inlineStr">
@@ -2830,7 +3989,102 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="AJ15" s="3" t="inlineStr"/>
+      <c r="AJ15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AK15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AL15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AM15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AN15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AO15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AP15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AQ15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AR15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AS15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AT15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AU15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AV15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AW15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AX15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AY15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="AZ15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BA15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BB15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BC15" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>

<commit_message>
feat(command) : add a command gathercolumn corresponding to the new function.
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_column_set_answer.xlsx
+++ b/fichiers_xls/test_column_set_answer.xlsx
@@ -462,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:BC15"/>
+  <dimension ref="A1:BF15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -757,6 +757,21 @@
       </c>
       <c r="BC2" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BD2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BE2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BF2" s="3" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -1032,6 +1047,21 @@
       </c>
       <c r="BC3" s="3" t="inlineStr">
         <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BD3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BE3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BF3" s="3" t="inlineStr">
+        <is>
           <t>9</t>
         </is>
       </c>
@@ -1307,6 +1337,21 @@
       </c>
       <c r="BC4" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BD4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BE4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BF4" s="3" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
@@ -1582,6 +1627,21 @@
       </c>
       <c r="BC5" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BD5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BE5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BF5" s="3" t="inlineStr">
+        <is>
           <t>10</t>
         </is>
       </c>
@@ -1855,7 +1915,22 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="BC6" s="3" t="inlineStr"/>
+      <c r="BC6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BD6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BE6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BF6" s="3" t="inlineStr"/>
     </row>
     <row r="7" ht="16.05" customHeight="1" s="4">
       <c r="A7" s="3" t="inlineStr">
@@ -2126,7 +2201,22 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="BC7" s="3" t="inlineStr"/>
+      <c r="BC7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BD7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BE7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BF7" s="3" t="inlineStr"/>
     </row>
     <row r="8" ht="16.05" customHeight="1" s="4">
       <c r="A8" s="3" t="inlineStr">
@@ -2397,7 +2487,22 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BC8" s="3" t="inlineStr"/>
+      <c r="BC8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BD8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BE8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BF8" s="3" t="inlineStr"/>
     </row>
     <row r="9" ht="16.05" customHeight="1" s="4">
       <c r="A9" s="3" t="inlineStr">
@@ -2668,7 +2773,22 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BC9" s="3" t="inlineStr"/>
+      <c r="BC9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BD9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BE9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BF9" s="3" t="inlineStr"/>
     </row>
     <row r="10" ht="16.05" customHeight="1" s="4">
       <c r="A10" s="3" t="inlineStr">
@@ -2730,6 +2850,9 @@
       <c r="BA10" s="3" t="inlineStr"/>
       <c r="BB10" s="3" t="inlineStr"/>
       <c r="BC10" s="3" t="inlineStr"/>
+      <c r="BD10" s="3" t="inlineStr"/>
+      <c r="BE10" s="3" t="inlineStr"/>
+      <c r="BF10" s="3" t="inlineStr"/>
     </row>
     <row r="11" ht="16.05" customHeight="1" s="4">
       <c r="A11" s="3" t="inlineStr">
@@ -3000,7 +3123,22 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BC11" s="3" t="inlineStr"/>
+      <c r="BC11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BD11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BE11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BF11" s="3" t="inlineStr"/>
     </row>
     <row r="12" ht="16.05" customHeight="1" s="4">
       <c r="A12" s="3" t="inlineStr">
@@ -3271,7 +3409,22 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BC12" s="3" t="inlineStr"/>
+      <c r="BC12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BD12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BE12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BF12" s="3" t="inlineStr"/>
     </row>
     <row r="13" ht="16.05" customHeight="1" s="4">
       <c r="A13" s="3" t="inlineStr">
@@ -3542,7 +3695,22 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BC13" s="3" t="inlineStr"/>
+      <c r="BC13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BD13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BE13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BF13" s="3" t="inlineStr"/>
     </row>
     <row r="14" ht="16.05" customHeight="1" s="4">
       <c r="A14" s="5" t="inlineStr">
@@ -3813,7 +3981,22 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BC14" s="3" t="inlineStr"/>
+      <c r="BC14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BD14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BE14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BF14" s="3" t="inlineStr"/>
     </row>
     <row r="15" ht="16.05" customHeight="1" s="4">
       <c r="A15" s="5" t="inlineStr">
@@ -4084,7 +4267,22 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="BC15" s="3" t="inlineStr"/>
+      <c r="BC15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BD15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BE15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BF15" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>

<commit_message>
feat(utils,command) : add two functions rangeLetter and listFromColumnsStrings to improve gathercolums.
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_column_set_answer.xlsx
+++ b/fichiers_xls/test_column_set_answer.xlsx
@@ -462,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:BF15"/>
+  <dimension ref="A1:BJ15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -772,6 +772,26 @@
       </c>
       <c r="BF2" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BG2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BH2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BI2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BJ2" s="3" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -1062,6 +1082,26 @@
       </c>
       <c r="BF3" s="3" t="inlineStr">
         <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BG3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BH3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BI3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BJ3" s="3" t="inlineStr">
+        <is>
           <t>9</t>
         </is>
       </c>
@@ -1352,6 +1392,26 @@
       </c>
       <c r="BF4" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BG4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BH4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BI4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BJ4" s="3" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
@@ -1642,6 +1702,26 @@
       </c>
       <c r="BF5" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BG5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BH5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BI5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BJ5" s="3" t="inlineStr">
+        <is>
           <t>10</t>
         </is>
       </c>
@@ -1930,7 +2010,27 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="BF6" s="3" t="inlineStr"/>
+      <c r="BF6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BG6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BH6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BI6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BJ6" s="3" t="inlineStr"/>
     </row>
     <row r="7" ht="16.05" customHeight="1" s="4">
       <c r="A7" s="3" t="inlineStr">
@@ -2216,7 +2316,27 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="BF7" s="3" t="inlineStr"/>
+      <c r="BF7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BG7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BH7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BI7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BJ7" s="3" t="inlineStr"/>
     </row>
     <row r="8" ht="16.05" customHeight="1" s="4">
       <c r="A8" s="3" t="inlineStr">
@@ -2502,7 +2622,27 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BF8" s="3" t="inlineStr"/>
+      <c r="BF8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BG8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BH8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BI8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BJ8" s="3" t="inlineStr"/>
     </row>
     <row r="9" ht="16.05" customHeight="1" s="4">
       <c r="A9" s="3" t="inlineStr">
@@ -2788,7 +2928,27 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BF9" s="3" t="inlineStr"/>
+      <c r="BF9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BG9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BH9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BI9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BJ9" s="3" t="inlineStr"/>
     </row>
     <row r="10" ht="16.05" customHeight="1" s="4">
       <c r="A10" s="3" t="inlineStr">
@@ -2853,6 +3013,10 @@
       <c r="BD10" s="3" t="inlineStr"/>
       <c r="BE10" s="3" t="inlineStr"/>
       <c r="BF10" s="3" t="inlineStr"/>
+      <c r="BG10" s="3" t="inlineStr"/>
+      <c r="BH10" s="3" t="inlineStr"/>
+      <c r="BI10" s="3" t="inlineStr"/>
+      <c r="BJ10" s="3" t="inlineStr"/>
     </row>
     <row r="11" ht="16.05" customHeight="1" s="4">
       <c r="A11" s="3" t="inlineStr">
@@ -3138,7 +3302,27 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BF11" s="3" t="inlineStr"/>
+      <c r="BF11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BG11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BH11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BI11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BJ11" s="3" t="inlineStr"/>
     </row>
     <row r="12" ht="16.05" customHeight="1" s="4">
       <c r="A12" s="3" t="inlineStr">
@@ -3424,7 +3608,27 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BF12" s="3" t="inlineStr"/>
+      <c r="BF12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BG12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BH12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BI12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BJ12" s="3" t="inlineStr"/>
     </row>
     <row r="13" ht="16.05" customHeight="1" s="4">
       <c r="A13" s="3" t="inlineStr">
@@ -3710,7 +3914,27 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BF13" s="3" t="inlineStr"/>
+      <c r="BF13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BG13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BH13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BI13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BJ13" s="3" t="inlineStr"/>
     </row>
     <row r="14" ht="16.05" customHeight="1" s="4">
       <c r="A14" s="5" t="inlineStr">
@@ -3996,7 +4220,27 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BF14" s="3" t="inlineStr"/>
+      <c r="BF14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BG14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BH14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BI14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BJ14" s="3" t="inlineStr"/>
     </row>
     <row r="15" ht="16.05" customHeight="1" s="4">
       <c r="A15" s="5" t="inlineStr">
@@ -4282,7 +4526,27 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="BF15" s="3" t="inlineStr"/>
+      <c r="BF15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BG15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BH15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BI15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BJ15" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>

<commit_message>
feat (mpe, command) : add the possibility to add a json file containig the mailing list for cutsendmail
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_column_set_answer.xlsx
+++ b/fichiers_xls/test_column_set_answer.xlsx
@@ -462,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:BO15"/>
+  <dimension ref="A1:BP15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -817,6 +817,11 @@
       </c>
       <c r="BO2" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BP2" s="3" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -1152,6 +1157,11 @@
       </c>
       <c r="BO3" s="3" t="inlineStr">
         <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BP3" s="3" t="inlineStr">
+        <is>
           <t>9</t>
         </is>
       </c>
@@ -1487,6 +1497,11 @@
       </c>
       <c r="BO4" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BP4" s="3" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
@@ -1822,6 +1837,11 @@
       </c>
       <c r="BO5" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BP5" s="3" t="inlineStr">
+        <is>
           <t>10</t>
         </is>
       </c>
@@ -2155,7 +2175,12 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="BO6" s="3" t="inlineStr"/>
+      <c r="BO6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BP6" s="3" t="inlineStr"/>
     </row>
     <row r="7" ht="16.05" customHeight="1" s="4">
       <c r="A7" s="3" t="inlineStr">
@@ -2486,7 +2511,12 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="BO7" s="3" t="inlineStr"/>
+      <c r="BO7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BP7" s="3" t="inlineStr"/>
     </row>
     <row r="8" ht="16.05" customHeight="1" s="4">
       <c r="A8" s="3" t="inlineStr">
@@ -2817,7 +2847,12 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BO8" s="3" t="inlineStr"/>
+      <c r="BO8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BP8" s="3" t="inlineStr"/>
     </row>
     <row r="9" ht="16.05" customHeight="1" s="4">
       <c r="A9" s="3" t="inlineStr">
@@ -3148,7 +3183,12 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BO9" s="3" t="inlineStr"/>
+      <c r="BO9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BP9" s="3" t="inlineStr"/>
     </row>
     <row r="10" ht="16.05" customHeight="1" s="4">
       <c r="A10" s="3" t="inlineStr">
@@ -3222,6 +3262,7 @@
       <c r="BM10" s="3" t="inlineStr"/>
       <c r="BN10" s="3" t="inlineStr"/>
       <c r="BO10" s="3" t="inlineStr"/>
+      <c r="BP10" s="3" t="inlineStr"/>
     </row>
     <row r="11" ht="16.05" customHeight="1" s="4">
       <c r="A11" s="3" t="inlineStr">
@@ -3552,7 +3593,12 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BO11" s="3" t="inlineStr"/>
+      <c r="BO11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BP11" s="3" t="inlineStr"/>
     </row>
     <row r="12" ht="16.05" customHeight="1" s="4">
       <c r="A12" s="3" t="inlineStr">
@@ -3883,7 +3929,12 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BO12" s="3" t="inlineStr"/>
+      <c r="BO12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BP12" s="3" t="inlineStr"/>
     </row>
     <row r="13" ht="16.05" customHeight="1" s="4">
       <c r="A13" s="3" t="inlineStr">
@@ -4214,7 +4265,12 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BO13" s="3" t="inlineStr"/>
+      <c r="BO13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BP13" s="3" t="inlineStr"/>
     </row>
     <row r="14" ht="16.05" customHeight="1" s="4">
       <c r="A14" s="5" t="inlineStr">
@@ -4545,7 +4601,12 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BO14" s="3" t="inlineStr"/>
+      <c r="BO14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BP14" s="3" t="inlineStr"/>
     </row>
     <row r="15" ht="16.05" customHeight="1" s="4">
       <c r="A15" s="5" t="inlineStr">
@@ -4876,7 +4937,12 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="BO15" s="3" t="inlineStr"/>
+      <c r="BO15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BP15" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>

<commit_message>
feat(sheet) : add the function give_names_of_maximum and the corresponding command maxnames
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_column_set_answer.xlsx
+++ b/fichiers_xls/test_column_set_answer.xlsx
@@ -462,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:BP15"/>
+  <dimension ref="A1:CB15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -822,6 +822,66 @@
       </c>
       <c r="BP2" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BQ2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BR2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BS2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BT2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BU2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BV2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BW2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BX2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BY2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BZ2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CA2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CB2" s="3" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -1162,6 +1222,66 @@
       </c>
       <c r="BP3" s="3" t="inlineStr">
         <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BQ3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BR3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BS3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BT3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BU3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BV3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BW3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BX3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BY3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BZ3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CA3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CB3" s="3" t="inlineStr">
+        <is>
           <t>9</t>
         </is>
       </c>
@@ -1502,6 +1622,66 @@
       </c>
       <c r="BP4" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BQ4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BR4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BS4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BT4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BU4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BV4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BW4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BX4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BY4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BZ4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CA4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CB4" s="3" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
@@ -1842,6 +2022,66 @@
       </c>
       <c r="BP5" s="3" t="inlineStr">
         <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BQ5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BR5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BS5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BT5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BU5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BV5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BW5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BX5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BY5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="BZ5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CA5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="CB5" s="3" t="inlineStr">
+        <is>
           <t>10</t>
         </is>
       </c>
@@ -2180,7 +2420,67 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="BP6" s="3" t="inlineStr"/>
+      <c r="BP6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BQ6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BR6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BS6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BT6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BU6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BV6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BW6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BX6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BY6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BZ6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CA6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CB6" s="3" t="inlineStr"/>
     </row>
     <row r="7" ht="16.05" customHeight="1" s="4">
       <c r="A7" s="3" t="inlineStr">
@@ -2516,7 +2816,67 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="BP7" s="3" t="inlineStr"/>
+      <c r="BP7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BQ7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BR7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BS7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BT7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BU7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BV7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BW7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BX7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BY7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BZ7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CA7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CB7" s="3" t="inlineStr"/>
     </row>
     <row r="8" ht="16.05" customHeight="1" s="4">
       <c r="A8" s="3" t="inlineStr">
@@ -2852,7 +3212,67 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BP8" s="3" t="inlineStr"/>
+      <c r="BP8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BQ8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BR8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BS8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BT8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BU8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BV8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BW8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BX8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BY8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BZ8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CA8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CB8" s="3" t="inlineStr"/>
     </row>
     <row r="9" ht="16.05" customHeight="1" s="4">
       <c r="A9" s="3" t="inlineStr">
@@ -3188,7 +3608,67 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BP9" s="3" t="inlineStr"/>
+      <c r="BP9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BQ9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BR9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BS9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BT9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BU9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BV9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BW9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BX9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BY9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BZ9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CA9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CB9" s="3" t="inlineStr"/>
     </row>
     <row r="10" ht="16.05" customHeight="1" s="4">
       <c r="A10" s="3" t="inlineStr">
@@ -3263,6 +3743,18 @@
       <c r="BN10" s="3" t="inlineStr"/>
       <c r="BO10" s="3" t="inlineStr"/>
       <c r="BP10" s="3" t="inlineStr"/>
+      <c r="BQ10" s="3" t="inlineStr"/>
+      <c r="BR10" s="3" t="inlineStr"/>
+      <c r="BS10" s="3" t="inlineStr"/>
+      <c r="BT10" s="3" t="inlineStr"/>
+      <c r="BU10" s="3" t="inlineStr"/>
+      <c r="BV10" s="3" t="inlineStr"/>
+      <c r="BW10" s="3" t="inlineStr"/>
+      <c r="BX10" s="3" t="inlineStr"/>
+      <c r="BY10" s="3" t="inlineStr"/>
+      <c r="BZ10" s="3" t="inlineStr"/>
+      <c r="CA10" s="3" t="inlineStr"/>
+      <c r="CB10" s="3" t="inlineStr"/>
     </row>
     <row r="11" ht="16.05" customHeight="1" s="4">
       <c r="A11" s="3" t="inlineStr">
@@ -3598,7 +4090,67 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BP11" s="3" t="inlineStr"/>
+      <c r="BP11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BQ11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BR11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BS11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BT11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BU11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BV11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BW11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BX11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BY11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BZ11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CA11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CB11" s="3" t="inlineStr"/>
     </row>
     <row r="12" ht="16.05" customHeight="1" s="4">
       <c r="A12" s="3" t="inlineStr">
@@ -3934,7 +4486,67 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BP12" s="3" t="inlineStr"/>
+      <c r="BP12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BQ12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BR12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BS12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BT12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BU12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BV12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BW12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BX12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BY12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BZ12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CA12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CB12" s="3" t="inlineStr"/>
     </row>
     <row r="13" ht="16.05" customHeight="1" s="4">
       <c r="A13" s="3" t="inlineStr">
@@ -4270,7 +4882,67 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BP13" s="3" t="inlineStr"/>
+      <c r="BP13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BQ13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BR13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BS13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BT13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BU13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BV13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BW13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BX13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BY13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BZ13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CA13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CB13" s="3" t="inlineStr"/>
     </row>
     <row r="14" ht="16.05" customHeight="1" s="4">
       <c r="A14" s="5" t="inlineStr">
@@ -4606,7 +5278,67 @@
           <t>group2</t>
         </is>
       </c>
-      <c r="BP14" s="3" t="inlineStr"/>
+      <c r="BP14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BQ14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BR14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BS14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BT14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BU14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BV14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BW14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BX14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BY14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="BZ14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CA14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="CB14" s="3" t="inlineStr"/>
     </row>
     <row r="15" ht="16.05" customHeight="1" s="4">
       <c r="A15" s="5" t="inlineStr">
@@ -4942,7 +5674,67 @@
           <t>group1</t>
         </is>
       </c>
-      <c r="BP15" s="3" t="inlineStr"/>
+      <c r="BP15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BQ15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BR15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BS15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BT15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BU15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BV15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BW15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BX15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BY15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="BZ15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CA15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="CB15" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>

<commit_message>
factor(xlspython): end of factorisation
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_column_set_answer.xlsx
+++ b/fichiers_xls/test_column_set_answer.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -354,16 +354,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.2734375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.2734375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col width="11.52" customWidth="1" style="3" min="645" max="1007"/>
-    <col width="11.53" customWidth="1" style="3" min="16368" max="16384"/>
+    <col width="11.52" customWidth="1" style="3" min="643" max="1005"/>
+    <col width="11.53" customWidth="1" style="3" min="16366" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" s="4">
@@ -389,16 +389,11 @@
           <t>1</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>group3</t>
-        </is>
-      </c>
-      <c r="D2" s="3">
-        <f>G2</f>
-        <v/>
-      </c>
-      <c r="G2" s="3" t="n">
+      <c r="C2" s="3">
+        <f>F2</f>
+        <v/>
+      </c>
+      <c r="F2" s="3" t="n">
         <v>12</v>
       </c>
     </row>
@@ -411,16 +406,11 @@
       <c r="B3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>group1</t>
-        </is>
-      </c>
-      <c r="D3" s="3">
-        <f>G3</f>
-        <v/>
-      </c>
-      <c r="G3" s="3" t="n">
+      <c r="C3" s="3">
+        <f>F3</f>
+        <v/>
+      </c>
+      <c r="F3" s="3" t="n">
         <v>13</v>
       </c>
     </row>
@@ -433,16 +423,11 @@
       <c r="B4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>group3</t>
-        </is>
-      </c>
-      <c r="D4" s="3">
-        <f>G4</f>
-        <v/>
-      </c>
-      <c r="G4" s="3" t="n">
+      <c r="C4" s="3">
+        <f>F4</f>
+        <v/>
+      </c>
+      <c r="F4" s="3" t="n">
         <v>14</v>
       </c>
     </row>
@@ -455,16 +440,11 @@
       <c r="B5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>group3</t>
-        </is>
-      </c>
-      <c r="D5" s="3">
-        <f>G5</f>
-        <v/>
-      </c>
-      <c r="G5" s="3" t="n">
+      <c r="C5" s="3">
+        <f>F5</f>
+        <v/>
+      </c>
+      <c r="F5" s="3" t="n">
         <v>15</v>
       </c>
     </row>
@@ -477,16 +457,11 @@
       <c r="B6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>group1</t>
-        </is>
-      </c>
-      <c r="D6" s="3">
-        <f>G6</f>
-        <v/>
-      </c>
-      <c r="G6" s="3" t="n">
+      <c r="C6" s="3">
+        <f>F6</f>
+        <v/>
+      </c>
+      <c r="F6" s="3" t="n">
         <v>16</v>
       </c>
     </row>
@@ -499,16 +474,11 @@
       <c r="B7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>group1</t>
-        </is>
-      </c>
-      <c r="D7" s="3">
-        <f>G7</f>
-        <v/>
-      </c>
-      <c r="G7" s="3" t="n">
+      <c r="C7" s="3">
+        <f>F7</f>
+        <v/>
+      </c>
+      <c r="F7" s="3" t="n">
         <v>17</v>
       </c>
     </row>
@@ -521,16 +491,11 @@
       <c r="B8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>group2</t>
-        </is>
-      </c>
-      <c r="D8" s="3">
-        <f>G8</f>
-        <v/>
-      </c>
-      <c r="G8" s="3" t="n">
+      <c r="C8" s="3">
+        <f>F8</f>
+        <v/>
+      </c>
+      <c r="F8" s="3" t="n">
         <v>18</v>
       </c>
     </row>
@@ -543,16 +508,11 @@
       <c r="B9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>group2</t>
-        </is>
-      </c>
-      <c r="D9" s="3">
-        <f>G9</f>
-        <v/>
-      </c>
-      <c r="G9" s="3" t="n">
+      <c r="C9" s="3">
+        <f>F9</f>
+        <v/>
+      </c>
+      <c r="F9" s="3" t="n">
         <v>19</v>
       </c>
     </row>
@@ -565,16 +525,11 @@
       <c r="B10" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>group2</t>
-        </is>
-      </c>
-      <c r="D10" s="3">
-        <f>G10</f>
-        <v/>
-      </c>
-      <c r="G10" s="3" t="n">
+      <c r="C10" s="3">
+        <f>F10</f>
+        <v/>
+      </c>
+      <c r="F10" s="3" t="n">
         <v>20</v>
       </c>
     </row>
@@ -587,16 +542,11 @@
       <c r="B11" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>group2</t>
-        </is>
-      </c>
-      <c r="D11" s="3">
-        <f>G11</f>
-        <v/>
-      </c>
-      <c r="G11" s="3" t="n">
+      <c r="C11" s="3">
+        <f>F11</f>
+        <v/>
+      </c>
+      <c r="F11" s="3" t="n">
         <v>21</v>
       </c>
     </row>
@@ -609,16 +559,11 @@
       <c r="B12" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>group2</t>
-        </is>
-      </c>
-      <c r="D12" s="3">
-        <f>G12</f>
-        <v/>
-      </c>
-      <c r="G12" s="3" t="n">
+      <c r="C12" s="3">
+        <f>F12</f>
+        <v/>
+      </c>
+      <c r="F12" s="3" t="n">
         <v>22</v>
       </c>
     </row>
@@ -631,16 +576,11 @@
       <c r="B13" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>group2</t>
-        </is>
-      </c>
-      <c r="D13" s="3">
-        <f>G13</f>
-        <v/>
-      </c>
-      <c r="G13" s="3" t="n">
+      <c r="C13" s="3">
+        <f>F13</f>
+        <v/>
+      </c>
+      <c r="F13" s="3" t="n">
         <v>23</v>
       </c>
     </row>
@@ -653,16 +593,11 @@
       <c r="B14" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>group2</t>
-        </is>
-      </c>
-      <c r="D14" s="3">
-        <f>G14</f>
-        <v/>
-      </c>
-      <c r="G14" s="3" t="n">
+      <c r="C14" s="3">
+        <f>F14</f>
+        <v/>
+      </c>
+      <c r="F14" s="3" t="n">
         <v>24</v>
       </c>
     </row>
@@ -675,16 +610,11 @@
       <c r="B15" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>group1</t>
-        </is>
-      </c>
-      <c r="D15" s="3">
-        <f>G15</f>
-        <v/>
-      </c>
-      <c r="G15" s="3" t="n">
+      <c r="C15" s="3">
+        <f>F15</f>
+        <v/>
+      </c>
+      <c r="F15" s="3" t="n">
         <v>25</v>
       </c>
     </row>
@@ -709,15 +639,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.2734375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.2734375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col width="11.53" customWidth="1" style="3" min="16381" max="16384"/>
+    <col width="11.53" customWidth="1" style="3" min="16382" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" s="4">
@@ -731,6 +661,7 @@
           <t>Prénom</t>
         </is>
       </c>
+      <c r="C1" s="3" t="n"/>
     </row>
     <row r="2" ht="15.75" customHeight="1" s="4">
       <c r="A2" s="3" t="inlineStr">
@@ -741,11 +672,16 @@
       <c r="B2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
-        <f>F2</f>
-        <v/>
-      </c>
-      <c r="F2" s="3" t="n">
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="D2" s="3">
+        <f>G2</f>
+        <v/>
+      </c>
+      <c r="G2" s="3" t="n">
         <v>12</v>
       </c>
     </row>
@@ -758,11 +694,16 @@
       <c r="B3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="3">
-        <f>F3</f>
-        <v/>
-      </c>
-      <c r="F3" s="3" t="n">
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="D3" s="3">
+        <f>G3</f>
+        <v/>
+      </c>
+      <c r="G3" s="3" t="n">
         <v>13</v>
       </c>
     </row>
@@ -775,11 +716,16 @@
       <c r="B4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="3">
-        <f>F4</f>
-        <v/>
-      </c>
-      <c r="F4" s="3" t="n">
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="D4" s="3">
+        <f>G4</f>
+        <v/>
+      </c>
+      <c r="G4" s="3" t="n">
         <v>14</v>
       </c>
     </row>
@@ -792,11 +738,16 @@
       <c r="B5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="3">
-        <f>F5</f>
-        <v/>
-      </c>
-      <c r="F5" s="3" t="n">
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>group3</t>
+        </is>
+      </c>
+      <c r="D5" s="3">
+        <f>G5</f>
+        <v/>
+      </c>
+      <c r="G5" s="3" t="n">
         <v>15</v>
       </c>
     </row>
@@ -809,11 +760,16 @@
       <c r="B6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="3">
-        <f>F6</f>
-        <v/>
-      </c>
-      <c r="F6" s="3" t="n">
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="D6" s="3">
+        <f>G6</f>
+        <v/>
+      </c>
+      <c r="G6" s="3" t="n">
         <v>16</v>
       </c>
     </row>
@@ -826,11 +782,16 @@
       <c r="B7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="C7" s="3">
-        <f>F7</f>
-        <v/>
-      </c>
-      <c r="F7" s="3" t="n">
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="D7" s="3">
+        <f>G7</f>
+        <v/>
+      </c>
+      <c r="G7" s="3" t="n">
         <v>17</v>
       </c>
     </row>
@@ -843,11 +804,16 @@
       <c r="B8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C8" s="3">
-        <f>F8</f>
-        <v/>
-      </c>
-      <c r="F8" s="3" t="n">
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="D8" s="3">
+        <f>G8</f>
+        <v/>
+      </c>
+      <c r="G8" s="3" t="n">
         <v>18</v>
       </c>
     </row>
@@ -860,11 +826,16 @@
       <c r="B9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C9" s="3">
-        <f>F9</f>
-        <v/>
-      </c>
-      <c r="F9" s="3" t="n">
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="D9" s="3">
+        <f>G9</f>
+        <v/>
+      </c>
+      <c r="G9" s="3" t="n">
         <v>19</v>
       </c>
     </row>
@@ -877,11 +848,16 @@
       <c r="B10" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C10" s="3">
-        <f>F10</f>
-        <v/>
-      </c>
-      <c r="F10" s="3" t="n">
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="D10" s="3">
+        <f>G10</f>
+        <v/>
+      </c>
+      <c r="G10" s="3" t="n">
         <v>20</v>
       </c>
     </row>
@@ -894,11 +870,16 @@
       <c r="B11" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C11" s="3">
-        <f>F11</f>
-        <v/>
-      </c>
-      <c r="F11" s="3" t="n">
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="D11" s="3">
+        <f>G11</f>
+        <v/>
+      </c>
+      <c r="G11" s="3" t="n">
         <v>21</v>
       </c>
     </row>
@@ -911,11 +892,16 @@
       <c r="B12" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C12" s="3">
-        <f>F12</f>
-        <v/>
-      </c>
-      <c r="F12" s="3" t="n">
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="D12" s="3">
+        <f>G12</f>
+        <v/>
+      </c>
+      <c r="G12" s="3" t="n">
         <v>22</v>
       </c>
     </row>
@@ -928,11 +914,16 @@
       <c r="B13" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C13" s="3">
-        <f>F13</f>
-        <v/>
-      </c>
-      <c r="F13" s="3" t="n">
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="D13" s="3">
+        <f>G13</f>
+        <v/>
+      </c>
+      <c r="G13" s="3" t="n">
         <v>23</v>
       </c>
     </row>
@@ -945,11 +936,16 @@
       <c r="B14" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="C14" s="3">
-        <f>F14</f>
-        <v/>
-      </c>
-      <c r="F14" s="3" t="n">
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
+      <c r="D14" s="3">
+        <f>G14</f>
+        <v/>
+      </c>
+      <c r="G14" s="3" t="n">
         <v>24</v>
       </c>
     </row>
@@ -962,11 +958,16 @@
       <c r="B15" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="C15" s="3">
-        <f>F15</f>
-        <v/>
-      </c>
-      <c r="F15" s="3" t="n">
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="D15" s="3">
+        <f>G15</f>
+        <v/>
+      </c>
+      <c r="G15" s="3" t="n">
         <v>25</v>
       </c>
     </row>

</xml_diff>